<commit_message>
began speccing voltage regulator
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.0-bom.xlsx
+++ b/sedani/estop/estop-1.0-bom.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFCDF5F-7DBD-4BA1-BE04-E0D5FB1BEB1C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4ED936-2A53-4468-A3D5-1DA7FAE09E09}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17544" windowHeight="10152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Part</t>
   </si>
@@ -35,6 +35,21 @@
   </si>
   <si>
     <t>3.3V regulator</t>
+  </si>
+  <si>
+    <t>10uH inductor</t>
+  </si>
+  <si>
+    <t>587-2886-1-ND</t>
+  </si>
+  <si>
+    <t>Needed</t>
+  </si>
+  <si>
+    <t>47uF ceramic</t>
+  </si>
+  <si>
+    <t>4.7uF ceramic</t>
   </si>
 </sst>
 </file>
@@ -352,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -364,7 +379,7 @@
     <col min="2" max="2" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -374,8 +389,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -384,6 +402,39 @@
       </c>
       <c r="C2">
         <v>1.23</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed crystal, finished voltage regulator, added LEDs
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.0-bom.xlsx
+++ b/sedani/estop/estop-1.0-bom.xlsx
@@ -1,15 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4ED936-2A53-4468-A3D5-1DA7FAE09E09}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE99019-6BEF-4EA9-BBFC-33F97DD4FF90}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4836" yWindow="1908" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Part</t>
   </si>
@@ -28,9 +31,6 @@
     <t>Number</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>296-39452-1-ND</t>
   </si>
   <si>
@@ -50,19 +50,79 @@
   </si>
   <si>
     <t>4.7uF ceramic</t>
+  </si>
+  <si>
+    <t>1k resistor</t>
+  </si>
+  <si>
+    <t>10k resistor</t>
+  </si>
+  <si>
+    <t>reset button</t>
+  </si>
+  <si>
+    <t>587-1780-1-ND</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Have</t>
+  </si>
+  <si>
+    <t>Unit Cost</t>
+  </si>
+  <si>
+    <t>401-1426-1-ND</t>
+  </si>
+  <si>
+    <t>541-3991-1-ND</t>
+  </si>
+  <si>
+    <t>0.1uF ceramic</t>
+  </si>
+  <si>
+    <t>ATMEGA32U4-AU</t>
+  </si>
+  <si>
+    <t>ATMEGA</t>
+  </si>
+  <si>
+    <t>1568-1394-ND</t>
+  </si>
+  <si>
+    <t>RFM69HCW - 915MHz</t>
+  </si>
+  <si>
+    <t>8MHz crystal</t>
+  </si>
+  <si>
+    <t>535-10212-1-ND</t>
+  </si>
+  <si>
+    <t>18pF ceramic cap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,8 +145,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -102,6 +164,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -367,19 +442,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,54 +463,149 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>4.12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>1.23</v>
-      </c>
-      <c r="D2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="D3">
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
+      <c r="E12" s="2">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added level shifter and button header. Need antenna
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.0-bom.xlsx
+++ b/sedani/estop/estop-1.0-bom.xlsx
@@ -3,16 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE99019-6BEF-4EA9-BBFC-33F97DD4FF90}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D9A155-A69A-42A0-9667-3D6C0A870AF0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4836" yWindow="1908" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Part</t>
   </si>
@@ -101,6 +98,12 @@
   </si>
   <si>
     <t>18pF ceramic cap</t>
+  </si>
+  <si>
+    <t>Level shifter</t>
+  </si>
+  <si>
+    <t>CD40109BPWR</t>
   </si>
 </sst>
 </file>
@@ -164,19 +167,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -442,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,6 +598,20 @@
         <v>2</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
changed output caps for 3.3V regulator
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.0-bom.xlsx
+++ b/sedani/estop/estop-1.0-bom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D9A155-A69A-42A0-9667-3D6C0A870AF0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74E97A3-3D34-4FC4-B6C7-DED3570E86BE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Part</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Needed</t>
   </si>
   <si>
-    <t>47uF ceramic</t>
-  </si>
-  <si>
     <t>4.7uF ceramic</t>
   </si>
   <si>
@@ -104,6 +101,12 @@
   </si>
   <si>
     <t>CD40109BPWR</t>
+  </si>
+  <si>
+    <t>732-8911-1-ND</t>
+  </si>
+  <si>
+    <t>220uF electrolytic</t>
   </si>
 </sst>
 </file>
@@ -435,7 +438,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,18 +459,18 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -478,10 +481,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -518,15 +521,21 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -537,29 +546,29 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -573,15 +582,15 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -592,7 +601,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -600,10 +609,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
       </c>
       <c r="C14">
         <v>1</v>

</xml_diff>

<commit_message>
made a SMA connector part
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.0-bom.xlsx
+++ b/sedani/estop/estop-1.0-bom.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74E97A3-3D34-4FC4-B6C7-DED3570E86BE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010D89EF-2790-47B3-AC46-B0A2D6A207C0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24750" yWindow="2985" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Part</t>
   </si>
@@ -100,13 +100,19 @@
     <t>Level shifter</t>
   </si>
   <si>
-    <t>CD40109BPWR</t>
-  </si>
-  <si>
     <t>732-8911-1-ND</t>
   </si>
   <si>
     <t>220uF electrolytic</t>
+  </si>
+  <si>
+    <t>SMA connector</t>
+  </si>
+  <si>
+    <t>CON-SMA-EDGE-S-ND</t>
+  </si>
+  <si>
+    <t>296-12163-1-ND</t>
   </si>
 </sst>
 </file>
@@ -435,16 +441,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.44140625" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
@@ -521,10 +527,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -612,13 +618,27 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="E14" s="2">
         <v>0.43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new connector to BOM but NOT SCHEMATIC
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.0-bom.xlsx
+++ b/sedani/estop/estop-1.0-bom.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F241811-7A1F-4A03-B714-F9F4F5BC7776}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55522746-ECE4-418F-8B81-1E835A44CA37}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24750" yWindow="2985" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -109,10 +109,10 @@
     <t>SMA connector</t>
   </si>
   <si>
-    <t>CON-SMA-EDGE-S-ND</t>
-  </si>
-  <si>
     <t>296-12163-1-ND</t>
+  </si>
+  <si>
+    <t>A97594-ND</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,7 +618,7 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -632,13 +632,13 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="E15" s="2">
-        <v>1.74</v>
+        <v>2.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed antenna to right angle and removed crystal
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.0-bom.xlsx
+++ b/sedani/estop/estop-1.0-bom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55522746-ECE4-418F-8B81-1E835A44CA37}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23998A15-BC88-4EEB-821B-CB5494938D29}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Part</t>
   </si>
@@ -88,24 +88,9 @@
     <t>RFM69HCW - 915MHz</t>
   </si>
   <si>
-    <t>8MHz crystal</t>
-  </si>
-  <si>
-    <t>535-10212-1-ND</t>
-  </si>
-  <si>
-    <t>18pF ceramic cap</t>
-  </si>
-  <si>
     <t>Level shifter</t>
   </si>
   <si>
-    <t>732-8911-1-ND</t>
-  </si>
-  <si>
-    <t>220uF electrolytic</t>
-  </si>
-  <si>
     <t>SMA connector</t>
   </si>
   <si>
@@ -113,6 +98,9 @@
   </si>
   <si>
     <t>A97594-ND</t>
+  </si>
+  <si>
+    <t>47uF ceramic</t>
   </si>
 </sst>
 </file>
@@ -441,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,13 +515,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -543,9 +534,6 @@
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
       <c r="E7" s="2">
         <v>0.7</v>
       </c>
@@ -596,48 +584,26 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="E12" s="2">
-        <v>0.27</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
       </c>
       <c r="C13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
         <v>2.17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added switch part numbers to BOM
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.0-bom.xlsx
+++ b/sedani/estop/estop-1.0-bom.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23998A15-BC88-4EEB-821B-CB5494938D29}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33A129C-712D-4359-AF5C-DCA03BB06DFC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
-  <si>
-    <t>Part</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>296-39452-1-ND</t>
   </si>
@@ -101,6 +95,60 @@
   </si>
   <si>
     <t>47uF ceramic</t>
+  </si>
+  <si>
+    <t>Off-board parts</t>
+  </si>
+  <si>
+    <t>On-board parts</t>
+  </si>
+  <si>
+    <t>Power switch</t>
+  </si>
+  <si>
+    <t>EG5617-ND</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>Other switch</t>
+  </si>
+  <si>
+    <t>CWI335-ND</t>
+  </si>
+  <si>
+    <t>Go button</t>
+  </si>
+  <si>
+    <t>CW232-ND</t>
+  </si>
+  <si>
+    <t>Stop button</t>
+  </si>
+  <si>
+    <t>CW233-ND</t>
+  </si>
+  <si>
+    <t>Right-angle antenna</t>
+  </si>
+  <si>
+    <t>DELTA2A/X/SMAM/S/RA/11-ND</t>
+  </si>
+  <si>
+    <t>Straight antenna</t>
+  </si>
+  <si>
+    <t>Right-angle SMA cable</t>
+  </si>
+  <si>
+    <t>Probalby not using</t>
+  </si>
+  <si>
+    <t>CBA-SMAMR-SMAF-ND</t>
+  </si>
+  <si>
+    <t>Too long</t>
   </si>
 </sst>
 </file>
@@ -429,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,57 +488,104 @@
     <col min="1" max="1" width="21.44140625" customWidth="1"/>
     <col min="2" max="2" width="18.77734375" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="2"/>
+    <col min="8" max="8" width="19.6640625" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4.12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2" s="2">
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3" s="2">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>4.12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="E3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -498,13 +593,28 @@
       <c r="E4" s="2">
         <v>1.23</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -512,13 +622,28 @@
       <c r="E5" s="2">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -526,43 +651,67 @@
       <c r="E6" s="2">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="M6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2">
+        <v>6.81</v>
+      </c>
+      <c r="M7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="F9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -574,17 +723,17 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
         <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -593,18 +742,37 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="E13" s="2">
         <v>2.17</v>
+      </c>
+    </row>
+    <row r="23" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H24" t="s">
+        <v>36</v>
+      </c>
+      <c r="I24" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="L24" s="2">
+        <v>10.82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added lipo charger to BOM
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.0-bom.xlsx
+++ b/sedani/estop/estop-1.0-bom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33A129C-712D-4359-AF5C-DCA03BB06DFC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49830C7D-A177-4A99-AFE0-809A889C4979}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>296-39452-1-ND</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t>Too long</t>
+  </si>
+  <si>
+    <t>LiPo charger</t>
+  </si>
+  <si>
+    <t>Look for alternative</t>
+  </si>
+  <si>
+    <t>adafruit.com/product/1944</t>
   </si>
 </sst>
 </file>
@@ -158,7 +167,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +180,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -190,15 +207,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -480,7 +500,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,6 +511,7 @@
     <col min="8" max="8" width="19.6640625" customWidth="1"/>
     <col min="9" max="9" width="27.33203125" customWidth="1"/>
     <col min="12" max="12" width="8.88671875" style="2"/>
+    <col min="13" max="13" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -694,6 +715,21 @@
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2">
+        <v>14.95</v>
+      </c>
+      <c r="M8" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -776,7 +812,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I8" r:id="rId1" display="www.adafruit.com/product/259" xr:uid="{D137116E-410B-4C1A-B8AB-EB48CC712A39}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added terminal blocks to BOM and tweaked documentation
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.0-bom.xlsx
+++ b/sedani/estop/estop-1.0-bom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49830C7D-A177-4A99-AFE0-809A889C4979}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB83A082-2509-46B6-8394-D77174EF9520}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>296-39452-1-ND</t>
   </si>
@@ -154,17 +154,30 @@
     <t>LiPo charger</t>
   </si>
   <si>
-    <t>Look for alternative</t>
-  </si>
-  <si>
     <t>adafruit.com/product/1944</t>
+  </si>
+  <si>
+    <t>2000 mAh LiPo</t>
+  </si>
+  <si>
+    <t>adafruit.com/product/2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.adafruit.com/product/724 </t>
+  </si>
+  <si>
+    <t>1 pack</t>
+  </si>
+  <si>
+    <t>Screw terminals for LiPo charger</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -211,11 +224,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -500,75 +525,79 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="1"/>
     <col min="5" max="5" width="8.88671875" style="2"/>
-    <col min="8" max="8" width="19.6640625" customWidth="1"/>
-    <col min="9" max="9" width="27.33203125" customWidth="1"/>
+    <col min="6" max="7" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="19.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="8.88671875" style="1"/>
     <col min="12" max="12" width="8.88671875" style="2"/>
-    <col min="13" max="13" width="17.5546875" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="2">
         <v>4.12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
         <v>2</v>
       </c>
       <c r="L2" s="2">
@@ -576,25 +605,25 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
         <v>2</v>
       </c>
       <c r="L3" s="2">
@@ -602,28 +631,28 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="2">
         <v>1.23</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
         <v>2</v>
       </c>
       <c r="L4" s="2">
@@ -631,28 +660,28 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
         <v>2</v>
       </c>
       <c r="L5" s="2">
@@ -660,118 +689,139 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="2">
         <v>0.7</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <v>2</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="2">
         <v>0.7</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="1">
         <v>1</v>
       </c>
       <c r="L7" s="2">
         <v>6.81</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8">
+      <c r="I8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="1">
         <v>1</v>
       </c>
       <c r="L8" s="2">
         <v>14.95</v>
       </c>
-      <c r="M8" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>0</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="H9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
+      <c r="L9" s="2">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
         <v>2</v>
       </c>
       <c r="E10" s="2">
         <v>0.52</v>
       </c>
+      <c r="H10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" s="5">
+        <v>2.95</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="2">
@@ -779,13 +829,13 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>1</v>
       </c>
       <c r="E13" s="2">
@@ -793,18 +843,18 @@
       </c>
     </row>
     <row r="23" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H23" t="s">
+      <c r="H23" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="24" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H24" t="s">
+      <c r="H24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="1">
         <v>1</v>
       </c>
       <c r="L24" s="2">
@@ -814,8 +864,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I8" r:id="rId1" display="www.adafruit.com/product/259" xr:uid="{D137116E-410B-4C1A-B8AB-EB48CC712A39}"/>
+    <hyperlink ref="I9" r:id="rId2" display="www.adafruit.com/product/2011" xr:uid="{E42F21C1-0492-40EB-AEF7-53F2B2F5708E}"/>
+    <hyperlink ref="I10" r:id="rId3" xr:uid="{996DCB62-E088-4E61-914D-CC473C3C91A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed link problem in BOM
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.0-bom.xlsx
+++ b/sedani/estop/estop-1.0-bom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB83A082-2509-46B6-8394-D77174EF9520}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4554F462-7A78-4E3D-B6B0-008440BDDEF0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,9 +154,6 @@
     <t>LiPo charger</t>
   </si>
   <si>
-    <t>adafruit.com/product/1944</t>
-  </si>
-  <si>
     <t>2000 mAh LiPo</t>
   </si>
   <si>
@@ -170,6 +167,9 @@
   </si>
   <si>
     <t>Screw terminals for LiPo charger</t>
+  </si>
+  <si>
+    <t>www.adafruit.com/product/1944</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,7 +536,7 @@
     <col min="5" max="5" width="8.88671875" style="2"/>
     <col min="6" max="7" width="8.88671875" style="1"/>
     <col min="8" max="8" width="19.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="27.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.21875" style="1" customWidth="1"/>
     <col min="10" max="11" width="8.88671875" style="1"/>
     <col min="12" max="12" width="8.88671875" style="2"/>
     <col min="13" max="13" width="17.5546875" style="1" customWidth="1"/>
@@ -748,7 +748,7 @@
         <v>43</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="J8" s="1">
         <v>1</v>
@@ -768,10 +768,10 @@
         <v>11</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="J9" s="1">
         <v>1</v>
@@ -797,13 +797,13 @@
         <v>0.52</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="L10" s="5">
         <v>2.95</v>
@@ -863,9 +863,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I8" r:id="rId1" display="www.adafruit.com/product/259" xr:uid="{D137116E-410B-4C1A-B8AB-EB48CC712A39}"/>
-    <hyperlink ref="I9" r:id="rId2" display="www.adafruit.com/product/2011" xr:uid="{E42F21C1-0492-40EB-AEF7-53F2B2F5708E}"/>
-    <hyperlink ref="I10" r:id="rId3" xr:uid="{996DCB62-E088-4E61-914D-CC473C3C91A1}"/>
+    <hyperlink ref="I9" r:id="rId1" display="www.adafruit.com/product/2011" xr:uid="{E42F21C1-0492-40EB-AEF7-53F2B2F5708E}"/>
+    <hyperlink ref="I10" r:id="rId2" xr:uid="{996DCB62-E088-4E61-914D-CC473C3C91A1}"/>
+    <hyperlink ref="I8" r:id="rId3" xr:uid="{F8FCF166-57E3-4B3F-A665-042561BF6934}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
fixed ground plane so it doesn't exceed board
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.0-bom.xlsx
+++ b/sedani/estop/estop-1.0-bom.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EC9053-D47E-49CF-ABD4-D37CC5523EE3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FBE4A7-2B71-4D17-AC88-1356ABD86407}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>296-39452-1-ND</t>
   </si>
@@ -40,9 +40,6 @@
     <t>4.7uF ceramic</t>
   </si>
   <si>
-    <t>1k resistor</t>
-  </si>
-  <si>
     <t>10k resistor</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>401-1426-1-ND</t>
   </si>
   <si>
-    <t>541-3991-1-ND</t>
-  </si>
-  <si>
     <t>0.1uF ceramic</t>
   </si>
   <si>
@@ -85,9 +79,6 @@
     <t>Level shifter</t>
   </si>
   <si>
-    <t>SMA connector</t>
-  </si>
-  <si>
     <t>296-12163-1-ND</t>
   </si>
   <si>
@@ -170,6 +161,24 @@
   </si>
   <si>
     <t>www.adafruit.com/product/1944</t>
+  </si>
+  <si>
+    <t>SMA right-angle panel mount connector</t>
+  </si>
+  <si>
+    <t>SMA PCB connector</t>
+  </si>
+  <si>
+    <t>SMA wire connectors</t>
+  </si>
+  <si>
+    <t>50 ohm SMA coax</t>
+  </si>
+  <si>
+    <t>330 ohm resistor</t>
+  </si>
+  <si>
+    <t>220 ohm resistor</t>
   </si>
 </sst>
 </file>
@@ -525,7 +534,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,42 +555,42 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -590,10 +599,10 @@
         <v>4.12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J2" s="1">
         <v>1</v>
@@ -607,19 +616,19 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J3" s="1">
         <v>1</v>
@@ -645,10 +654,10 @@
         <v>1.23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J4" s="1">
         <v>1</v>
@@ -674,10 +683,10 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J5" s="1">
         <v>1</v>
@@ -691,10 +700,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -703,13 +712,13 @@
         <v>0.7</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J6" s="1">
         <v>2</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -717,16 +726,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
         <v>0.7</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J7" s="1">
         <v>1</v>
@@ -735,21 +744,21 @@
         <v>6.81</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J8" s="1">
         <v>1</v>
@@ -760,19 +769,16 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>11</v>
+        <v>52</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J9" s="1">
         <v>1</v>
@@ -783,28 +789,20 @@
     </row>
     <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B10" s="3"/>
       <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.52</v>
+        <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L10" s="5">
         <v>2.95</v>
@@ -812,48 +810,95 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
       <c r="E12" s="2">
-        <v>0.43</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
       <c r="E13" s="2">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
         <v>2.17</v>
       </c>
     </row>
-    <row r="23" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H23" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="8:12" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H24" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J24" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
updated BOM. Ready for order for v1.0.
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.0-bom.xlsx
+++ b/sedani/estop/estop-1.0-bom.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FBE4A7-2B71-4D17-AC88-1356ABD86407}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F03C81E-687E-4A12-A464-2050F98EDBC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
   <si>
     <t>296-39452-1-ND</t>
   </si>
@@ -163,22 +169,55 @@
     <t>www.adafruit.com/product/1944</t>
   </si>
   <si>
-    <t>SMA right-angle panel mount connector</t>
-  </si>
-  <si>
     <t>SMA PCB connector</t>
   </si>
   <si>
-    <t>SMA wire connectors</t>
-  </si>
-  <si>
-    <t>50 ohm SMA coax</t>
-  </si>
-  <si>
     <t>330 ohm resistor</t>
   </si>
   <si>
     <t>220 ohm resistor</t>
+  </si>
+  <si>
+    <t>1276-1044-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1000-1-ND</t>
+  </si>
+  <si>
+    <t>1uF ceramic</t>
+  </si>
+  <si>
+    <t>10nF ceramic</t>
+  </si>
+  <si>
+    <t>1276-1866-1-ND</t>
+  </si>
+  <si>
+    <t>732-8007-1-ND</t>
+  </si>
+  <si>
+    <t>A130087CT-ND</t>
+  </si>
+  <si>
+    <t>CR0603-JW-331ELFCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603JT10K0CT-ND</t>
+  </si>
+  <si>
+    <t>Red 5mm THT LED</t>
+  </si>
+  <si>
+    <t>Blue 5mm THT LED</t>
+  </si>
+  <si>
+    <t>Yellow 5mm THT LED</t>
+  </si>
+  <si>
+    <t>Green 5mm THT LED</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
   </si>
 </sst>
 </file>
@@ -534,16 +573,16 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22" style="1" customWidth="1"/>
     <col min="3" max="4" width="8.88671875" style="1"/>
     <col min="5" max="5" width="8.88671875" style="2"/>
-    <col min="6" max="6" width="8.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" style="2" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" style="1"/>
     <col min="8" max="8" width="19.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="29.21875" style="1" customWidth="1"/>
@@ -569,6 +608,9 @@
       <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
@@ -593,10 +635,17 @@
         <v>14</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
       </c>
       <c r="E2" s="2">
         <v>4.12</v>
+      </c>
+      <c r="F2" s="2">
+        <f>D2*E2</f>
+        <v>12.36</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>29</v>
@@ -622,7 +671,17 @@
         <v>16</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5.95</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F16" si="0">D3*E3</f>
+        <v>17.850000000000001</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>31</v>
@@ -648,11 +707,18 @@
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
       </c>
       <c r="E4" s="2">
         <v>1.23</v>
       </c>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>3.69</v>
+      </c>
       <c r="H4" s="1" t="s">
         <v>24</v>
       </c>
@@ -677,10 +743,17 @@
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
       </c>
       <c r="E5" s="2">
         <v>0.28999999999999998</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.86999999999999988</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>27</v>
@@ -706,10 +779,17 @@
         <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
       </c>
       <c r="E6" s="2">
-        <v>0.7</v>
+        <v>0.67</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>2.0100000000000002</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>35</v>
@@ -725,11 +805,21 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
+      <c r="B7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
       </c>
       <c r="E7" s="2">
-        <v>0.7</v>
+        <v>0.15</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>36</v>
@@ -749,10 +839,23 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>52</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.34</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>40</v>
@@ -769,10 +872,23 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>41</v>
@@ -789,11 +905,23 @@
     </row>
     <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="C10" s="1">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.9E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.19</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>45</v>
@@ -810,90 +938,154 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>49</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="C11" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.21999999999999997</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>48</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="C12" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2">
-        <v>0.52</v>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>10</v>
       </c>
       <c r="E13" s="2">
-        <v>0.43</v>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
       </c>
       <c r="E14" s="2">
-        <v>2.17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.52</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>1.56</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>18</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>1.29</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2.17</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="0"/>
+        <v>6.51</v>
+      </c>
+    </row>
+    <row r="18" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F18" s="2">
+        <f>SUM(F2:F16)</f>
+        <v>48.269999999999989</v>
+      </c>
+    </row>
+    <row r="23" spans="6:12" x14ac:dyDescent="0.3">
       <c r="H23" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:12" x14ac:dyDescent="0.3">
       <c r="H24" s="1" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
finished BOM for e-stop remote and car
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.0-bom.xlsx
+++ b/sedani/estop/estop-1.0-bom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F03C81E-687E-4A12-A464-2050F98EDBC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841814DD-DFC3-4E59-9BAD-ECAF3E1921A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
   <si>
     <t>296-39452-1-ND</t>
   </si>
@@ -127,27 +127,15 @@
     <t>CW233-ND</t>
   </si>
   <si>
-    <t>Right-angle antenna</t>
-  </si>
-  <si>
-    <t>DELTA2A/X/SMAM/S/RA/11-ND</t>
-  </si>
-  <si>
     <t>Straight antenna</t>
   </si>
   <si>
     <t>Right-angle SMA cable</t>
   </si>
   <si>
-    <t>Probalby not using</t>
-  </si>
-  <si>
     <t>CBA-SMAMR-SMAF-ND</t>
   </si>
   <si>
-    <t>Too long</t>
-  </si>
-  <si>
     <t>LiPo charger</t>
   </si>
   <si>
@@ -160,12 +148,6 @@
     <t xml:space="preserve">www.adafruit.com/product/724 </t>
   </si>
   <si>
-    <t>1 pack</t>
-  </si>
-  <si>
-    <t>Screw terminals for LiPo charger</t>
-  </si>
-  <si>
     <t>www.adafruit.com/product/1944</t>
   </si>
   <si>
@@ -218,6 +200,48 @@
   </si>
   <si>
     <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Parts are for both remote and on-car boards</t>
+  </si>
+  <si>
+    <t>C503B-BAN-CY0C0461-ND</t>
+  </si>
+  <si>
+    <t>C503B-RAN-CA0C0AA1-ND</t>
+  </si>
+  <si>
+    <t>365-1183-ND</t>
+  </si>
+  <si>
+    <t>C503B-GAN-CB0F0791-ND</t>
+  </si>
+  <si>
+    <t>3.5mm Screw terminals for LiPo charger</t>
+  </si>
+  <si>
+    <t>2.5mm screw terminals for low batt light</t>
+  </si>
+  <si>
+    <t>www.adafruit.com/product/2134</t>
+  </si>
+  <si>
+    <t>9-pin screw terminal for PCB</t>
+  </si>
+  <si>
+    <t>Power out of charger</t>
+  </si>
+  <si>
+    <t>Low battery light</t>
+  </si>
+  <si>
+    <t>www.adafruit.com/product/2136</t>
+  </si>
+  <si>
+    <t>LoRa radio</t>
+  </si>
+  <si>
+    <t>1597-1488-ND</t>
   </si>
 </sst>
 </file>
@@ -570,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,15 +608,16 @@
     <col min="5" max="5" width="8.88671875" style="2"/>
     <col min="6" max="6" width="9.88671875" style="2" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" style="1"/>
-    <col min="8" max="8" width="19.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" style="1" customWidth="1"/>
     <col min="9" max="9" width="29.21875" style="1" customWidth="1"/>
     <col min="10" max="11" width="8.88671875" style="1"/>
     <col min="12" max="12" width="8.88671875" style="2"/>
     <col min="13" max="13" width="17.5546875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="18.77734375" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -609,7 +634,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>22</v>
@@ -626,8 +651,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -638,14 +666,14 @@
         <v>2</v>
       </c>
       <c r="D2" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2">
         <v>4.12</v>
       </c>
       <c r="F2" s="2">
         <f>D2*E2</f>
-        <v>12.36</v>
+        <v>8.24</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>29</v>
@@ -662,8 +690,12 @@
       <c r="L2" s="2">
         <v>2.84</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M2" s="2">
+        <f>K2*L2</f>
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -698,8 +730,12 @@
       <c r="L3" s="2">
         <v>2.77</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M3" s="2">
+        <f t="shared" ref="M3:M16" si="1">K3*L3</f>
+        <v>5.54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -734,8 +770,12 @@
       <c r="L4" s="2">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M4" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -770,8 +810,12 @@
       <c r="L5" s="2">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M5" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -792,21 +836,31 @@
         <v>2.0100000000000002</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>35</v>
+        <v>53</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="J6" s="1">
-        <v>2</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>2</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="1"/>
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
@@ -822,27 +876,31 @@
         <v>0.75</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="J7" s="1">
         <v>1</v>
       </c>
+      <c r="K7" s="1">
+        <v>2</v>
+      </c>
       <c r="L7" s="2">
-        <v>6.81</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -858,24 +916,31 @@
         <v>0.34</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>46</v>
+        <v>55</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="J8" s="1">
         <v>1</v>
       </c>
+      <c r="K8" s="1">
+        <v>2</v>
+      </c>
       <c r="L8" s="2">
-        <v>14.95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.2</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1">
         <v>6</v>
@@ -891,24 +956,31 @@
         <v>0.33</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="J9" s="1">
         <v>1</v>
       </c>
+      <c r="K9" s="1">
+        <v>2</v>
+      </c>
       <c r="L9" s="2">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.25</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -924,24 +996,25 @@
         <v>0.19</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L10" s="5">
-        <v>2.95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1">
         <v>4</v>
@@ -957,15 +1030,31 @@
         <v>0.21999999999999997</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2">
+        <v>6.81</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="1"/>
+        <v>6.81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1">
         <v>6</v>
@@ -981,15 +1070,31 @@
         <v>0.15</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2">
+        <v>14.95</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="1"/>
+        <v>14.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -1005,10 +1110,26 @@
         <v>0.15</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1">
+        <v>2</v>
+      </c>
+      <c r="L13" s="2">
+        <v>12.5</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1029,10 +1150,29 @@
         <v>1.56</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+      <c r="L14" s="5">
+        <v>2.95</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="1"/>
+        <v>2.95</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1052,10 +1192,32 @@
         <f t="shared" si="0"/>
         <v>1.29</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="1"/>
+        <v>1.25</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>20</v>
@@ -1073,39 +1235,61 @@
         <f t="shared" si="0"/>
         <v>6.51</v>
       </c>
-    </row>
-    <row r="18" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="H16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2">
+        <v>3.05</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="1"/>
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F18" s="2">
         <f>SUM(F2:F16)</f>
-        <v>48.269999999999989</v>
-      </c>
-    </row>
-    <row r="23" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="H23" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="H24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J24" s="1">
-        <v>1</v>
-      </c>
-      <c r="L24" s="2">
-        <v>10.82</v>
+        <v>44.15</v>
+      </c>
+      <c r="M18" s="2">
+        <f>SUM(M2:M16)</f>
+        <v>69.41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="2">
+        <v>7.66</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I9" r:id="rId1" display="www.adafruit.com/product/2011" xr:uid="{E42F21C1-0492-40EB-AEF7-53F2B2F5708E}"/>
-    <hyperlink ref="I10" r:id="rId2" xr:uid="{996DCB62-E088-4E61-914D-CC473C3C91A1}"/>
-    <hyperlink ref="I8" r:id="rId3" xr:uid="{F8FCF166-57E3-4B3F-A665-042561BF6934}"/>
+    <hyperlink ref="I13" r:id="rId1" display="www.adafruit.com/product/2011" xr:uid="{E42F21C1-0492-40EB-AEF7-53F2B2F5708E}"/>
+    <hyperlink ref="I14" r:id="rId2" xr:uid="{996DCB62-E088-4E61-914D-CC473C3C91A1}"/>
+    <hyperlink ref="I12" r:id="rId3" xr:uid="{F8FCF166-57E3-4B3F-A665-042561BF6934}"/>
+    <hyperlink ref="I15" r:id="rId4" xr:uid="{FBC8E941-7B24-4FAF-ACEB-DD0438F6BDD9}"/>
+    <hyperlink ref="I16" r:id="rId5" xr:uid="{47868E09-3EC4-42BC-8E64-F5105C27F835}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>